<commit_message>
TC_addNewCustomer completed with mysql bd
</commit_message>
<xml_diff>
--- a/src/main/java/testData/customers_data.xlsx
+++ b/src/main/java/testData/customers_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gurpreet Kooner\Projects\EclipseProjects\Projects\TestNetBanking\src\main\java\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEFE2028-3139-48AD-BAF7-FC787EC492B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A771ADF6-5631-4275-B750-6B3FC5FB0FCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -73,9 +73,6 @@
     <t>Delhi</t>
   </si>
   <si>
-    <t>plm@plk.com</t>
-  </si>
-  <si>
     <t>Rohan Walia</t>
   </si>
   <si>
@@ -83,9 +80,6 @@
 Shardha</t>
   </si>
   <si>
-    <t>okm@okj.com</t>
-  </si>
-  <si>
     <t>Kartik Pathak</t>
   </si>
   <si>
@@ -93,9 +87,6 @@
 Holi Mahal</t>
   </si>
   <si>
-    <t>ijh@wsk.com</t>
-  </si>
-  <si>
     <t>Sita Kumari</t>
   </si>
   <si>
@@ -106,9 +97,6 @@
 Mayur Vihar</t>
   </si>
   <si>
-    <t>oos@ggp.com</t>
-  </si>
-  <si>
     <t>Deepa</t>
   </si>
   <si>
@@ -116,9 +104,6 @@
 Mayur Vihar</t>
   </si>
   <si>
-    <t>asv@wer.com</t>
-  </si>
-  <si>
     <t>Komal</t>
   </si>
   <si>
@@ -126,9 +111,6 @@
 Pandav Vihar</t>
   </si>
   <si>
-    <t>qpl@snx.com</t>
-  </si>
-  <si>
     <t>01-01-2004</t>
   </si>
   <si>
@@ -148,6 +130,24 @@
   </si>
   <si>
     <t>110087</t>
+  </si>
+  <si>
+    <t>plhm@plaka.com</t>
+  </si>
+  <si>
+    <t>okmh@okaaj.com</t>
+  </si>
+  <si>
+    <t>ijhh@waska.com</t>
+  </si>
+  <si>
+    <t>oosh@gagap.com</t>
+  </si>
+  <si>
+    <t>asvh@waear.com</t>
+  </si>
+  <si>
+    <t>qplh@sanax.com</t>
   </si>
 </sst>
 </file>
@@ -189,12 +189,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -478,12 +475,13 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="J2" sqref="A2:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -519,7 +517,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -527,9 +525,9 @@
         <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -545,24 +543,24 @@
         <v>9876543210</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>28</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>13</v>
@@ -571,30 +569,30 @@
         <v>14</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="H3" s="1">
         <v>8765432190</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>20</v>
+        <v>29</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>13</v>
@@ -609,24 +607,24 @@
         <v>7654321980</v>
       </c>
       <c r="I4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>13</v>
@@ -641,24 +639,24 @@
         <v>6543210987</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>13</v>
@@ -673,24 +671,24 @@
         <v>5432109876</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>13</v>
@@ -705,14 +703,15 @@
         <v>4321098765</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>